<commit_message>
New template; there are levels.
Template based on <table> element.
</commit_message>
<xml_diff>
--- a/Exemple.xlsx
+++ b/Exemple.xlsx
@@ -7,25 +7,25 @@
     <workbookView xWindow="240" yWindow="90" windowWidth="19980" windowHeight="7815" tabRatio="628"/>
   </bookViews>
   <sheets>
-    <sheet name="Захід-школа" sheetId="1" r:id="rId1"/>
-    <sheet name="Захід-гімназія" sheetId="2" r:id="rId2"/>
-    <sheet name="Схід-школа" sheetId="3" r:id="rId3"/>
-    <sheet name="Схід-гімназія" sheetId="4" r:id="rId4"/>
-    <sheet name="Південь-школа" sheetId="5" r:id="rId5"/>
-    <sheet name="Південь-гімназія" sheetId="6" r:id="rId6"/>
-    <sheet name="Центр-школа" sheetId="7" r:id="rId7"/>
-    <sheet name="Центр-гімназія" sheetId="8" r:id="rId8"/>
-    <sheet name="Сімферополь-школа" sheetId="9" r:id="rId9"/>
-    <sheet name="Сімферополь-гімназія" sheetId="10" r:id="rId10"/>
-    <sheet name="Київ-школа" sheetId="11" r:id="rId11"/>
-    <sheet name="Київ-гімназія" sheetId="12" r:id="rId12"/>
+    <sheet name="Захід-1" sheetId="1" r:id="rId1"/>
+    <sheet name="Захід-2" sheetId="2" r:id="rId2"/>
+    <sheet name="Схід-1" sheetId="3" r:id="rId3"/>
+    <sheet name="Схід-2" sheetId="4" r:id="rId4"/>
+    <sheet name="Південь-1" sheetId="5" r:id="rId5"/>
+    <sheet name="Південь-2" sheetId="6" r:id="rId6"/>
+    <sheet name="Центр-1" sheetId="7" r:id="rId7"/>
+    <sheet name="Центр-2" sheetId="8" r:id="rId8"/>
+    <sheet name="Сімферополь-1" sheetId="9" r:id="rId9"/>
+    <sheet name="Сімферополь-2" sheetId="10" r:id="rId10"/>
+    <sheet name="Київ-1" sheetId="11" r:id="rId11"/>
+    <sheet name="Київ-2" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>7а</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>10в</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -16901,7 +16904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:143" ht="12.75">
+    <row r="41" spans="1:143">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -16921,7 +16924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:143" ht="12.75">
+    <row r="42" spans="1:143">
       <c r="B42">
         <v>1</v>
       </c>
@@ -17331,7 +17334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:143" ht="12.75">
+    <row r="43" spans="1:143">
       <c r="B43">
         <v>2</v>
       </c>
@@ -17744,7 +17747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:143" ht="12.75">
+    <row r="44" spans="1:143">
       <c r="B44">
         <v>1</v>
       </c>
@@ -18157,7 +18160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:143" ht="12.75">
+    <row r="45" spans="1:143">
       <c r="B45">
         <v>2</v>
       </c>
@@ -18567,7 +18570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:143" ht="12.75">
+    <row r="46" spans="1:143">
       <c r="B46">
         <v>2</v>
       </c>
@@ -19054,7 +19057,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19063,10 +19072,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19075,7 +19092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>